<commit_message>
Subscript industry CCS by energy related vs. process emissions (#129)
</commit_message>
<xml_diff>
--- a/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
+++ b/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ccs\CCP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\ccs\CCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458C486A-5B60-4A9B-B6D8-7B42A078F02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6405BF9F-1D3A-4C50-AE6F-24D97B944D8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="25020" windowHeight="14490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1575" yWindow="510" windowWidth="24540" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Source:</t>
   </si>
@@ -229,6 +229,12 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>energy related emissions</t>
+  </si>
+  <si>
+    <t>process emissions</t>
   </si>
 </sst>
 </file>
@@ -942,81 +948,113 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Switch to new industry categories in CPP/CPPbI (#89)
</commit_message>
<xml_diff>
--- a/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
+++ b/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\ccs\CCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6405BF9F-1D3A-4C50-AE6F-24D97B944D8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6134759D-C76E-400C-8C70-93E8AFC83C7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="510" windowWidth="24540" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21045" yWindow="1410" windowWidth="33360" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Source:</t>
   </si>
@@ -100,34 +100,7 @@
     <t>Unit: dimentionless (fraction of CO2 capturable)</t>
   </si>
   <si>
-    <t>cement and other carbonates</t>
-  </si>
-  <si>
-    <t>natural gas and petroleum systems</t>
-  </si>
-  <si>
-    <t>iron and steel</t>
-  </si>
-  <si>
-    <t>chemicals</t>
-  </si>
-  <si>
-    <t>mining</t>
-  </si>
-  <si>
-    <t>waste management</t>
-  </si>
-  <si>
-    <t>agriculture</t>
-  </si>
-  <si>
-    <t>other industries</t>
-  </si>
-  <si>
     <t>This variable should specify the share of CO2 emissions from each industry or power plant that could</t>
-  </si>
-  <si>
-    <t>For industries, we assign 100% to all industries except mining, agriculture, and waste management, as the activities</t>
   </si>
   <si>
     <t>in those industries are dispersed across areas (rather than concentrated inside machines in buildings) and in some cases,</t>
@@ -235,6 +208,87 @@
   </si>
   <si>
     <t>process emissions</t>
+  </si>
+  <si>
+    <t>agriculture and forestry 01T03</t>
+  </si>
+  <si>
+    <t>coal mining 05</t>
+  </si>
+  <si>
+    <t>oil and gas extraction 06</t>
+  </si>
+  <si>
+    <t>other mining and quarrying 07T08</t>
+  </si>
+  <si>
+    <t>food beverage and tobacco 10T12</t>
+  </si>
+  <si>
+    <t>textiles apparel and leather 13T15</t>
+  </si>
+  <si>
+    <t>wood products 16</t>
+  </si>
+  <si>
+    <t>pulp paper and printing 17T18</t>
+  </si>
+  <si>
+    <t>refined petroleum and coke 19</t>
+  </si>
+  <si>
+    <t>chemicals 20</t>
+  </si>
+  <si>
+    <t>rubber and plastic products 22</t>
+  </si>
+  <si>
+    <t>glass and glass products 231</t>
+  </si>
+  <si>
+    <t>cement and other nonmetallic minerals 239</t>
+  </si>
+  <si>
+    <t>iron and steel 241</t>
+  </si>
+  <si>
+    <t>other metals 242</t>
+  </si>
+  <si>
+    <t>metal products except machinery and vehicles 25</t>
+  </si>
+  <si>
+    <t>computers and electronics 26</t>
+  </si>
+  <si>
+    <t>appliances and electrical equipment 27</t>
+  </si>
+  <si>
+    <t>other machinery 28</t>
+  </si>
+  <si>
+    <t>road vehicles 29</t>
+  </si>
+  <si>
+    <t>nonroad vehicles 30</t>
+  </si>
+  <si>
+    <t>other manufacturing 31T33</t>
+  </si>
+  <si>
+    <t>energy pipelines and gas processing 352T353</t>
+  </si>
+  <si>
+    <t>water and waste 36T39</t>
+  </si>
+  <si>
+    <t>construction 41T43</t>
+  </si>
+  <si>
+    <t>For industries, we assign 100% to all industries except mining, agriculture, construction, and water and waste, as the activities</t>
+  </si>
+  <si>
+    <t>(We assume CO2 from "water and waste" is from waste collection trucks, not water treatment plants, which use almost entirely electricity.)</t>
   </si>
 </sst>
 </file>
@@ -659,7 +713,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -699,22 +753,22 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -725,7 +779,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -734,7 +788,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -743,45 +797,52 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
+      <c r="A23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -948,13 +1009,13 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
   </cols>
@@ -964,98 +1025,285 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split NG nonpeaker input data files outside electricity sheet (#232)
</commit_message>
<xml_diff>
--- a/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
+++ b/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\ccs\CCP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\ccs\CCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6134759D-C76E-400C-8C70-93E8AFC83C7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249BAD7E-E681-4E88-B4C2-E74CD19DF8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21045" yWindow="1410" windowWidth="33360" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16095" yWindow="1035" windowWidth="31950" windowHeight="21345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Source:</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>hard coal</t>
-  </si>
-  <si>
-    <t>natural gas nonpeaker</t>
   </si>
   <si>
     <t>nuclear</t>
@@ -289,6 +286,12 @@
   </si>
   <si>
     <t>(We assume CO2 from "water and waste" is from waste collection trucks, not water treatment plants, which use almost entirely electricity.)</t>
+  </si>
+  <si>
+    <t>natural gas steam turbine</t>
+  </si>
+  <si>
+    <t>natural gas combined cycle</t>
   </si>
 </sst>
 </file>
@@ -753,22 +756,22 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -779,7 +782,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -788,7 +791,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -797,21 +800,21 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -823,26 +826,26 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -856,7 +859,7 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -867,7 +870,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -880,7 +883,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -888,15 +891,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -904,7 +907,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -912,7 +915,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -920,7 +923,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -928,31 +931,31 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -960,7 +963,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -968,23 +971,23 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -992,9 +995,17 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
         <v>1</v>
       </c>
     </row>
@@ -1022,18 +1033,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1044,7 +1055,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1055,7 +1066,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1066,7 +1077,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1077,7 +1088,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1088,7 +1099,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1099,7 +1110,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1110,7 +1121,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1121,7 +1132,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1132,7 +1143,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1143,7 +1154,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1154,7 +1165,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1165,7 +1176,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1176,7 +1187,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1187,7 +1198,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1198,7 +1209,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1209,7 +1220,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1220,7 +1231,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1231,7 +1242,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1242,7 +1253,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1253,7 +1264,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1264,7 +1275,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1275,7 +1286,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1286,7 +1297,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1297,7 +1308,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26">
         <v>0</v>

</xml_diff>

<commit_message>
Modify electricity sector CCS tracking (issue #280)
</commit_message>
<xml_diff>
--- a/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
+++ b/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\CCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334B587A-BADD-4D46-93B6-4A898148B25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292B3CBC-45FD-45F3-A496-6285BA545B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -387,7 +387,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,7 +830,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A24"/>
+      <selection activeCell="B19" sqref="B19:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +848,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -857,7 +856,7 @@
         <v>61</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -865,7 +864,7 @@
         <v>62</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -913,7 +912,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -929,7 +928,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -937,7 +936,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -945,7 +944,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -961,7 +960,7 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -969,7 +968,7 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -977,55 +976,55 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
+      <c r="B19">
+        <v>0.95</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
+      <c r="B20">
+        <v>0.95</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="2">
-        <v>1</v>
+      <c r="B21">
+        <v>0.95</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="2">
-        <v>1</v>
+      <c r="B22">
+        <v>0.95</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="2">
-        <v>1</v>
+      <c r="B23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="2">
-        <v>1</v>
+      <c r="B24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add incremental demand for green hydrogen to RPS and begin adding blue hydrogen to CCS module
</commit_message>
<xml_diff>
--- a/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
+++ b/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\CCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB242916-3486-4863-B65A-1BC02A5C7437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7172B8-79FD-4360-98F3-E9249B18DB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="CPPbES" sheetId="12" r:id="rId2"/>
     <sheet name="CPPbI" sheetId="13" r:id="rId3"/>
+    <sheet name="CPPbHS" sheetId="15" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>Source:</t>
   </si>
@@ -313,6 +314,12 @@
   </si>
   <si>
     <t>hydrogen combined cycle</t>
+  </si>
+  <si>
+    <t>natural gas reforming with CCS</t>
+  </si>
+  <si>
+    <t>capture rate</t>
   </si>
 </sst>
 </file>
@@ -1359,4 +1366,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D48B9D0-7C8A-4023-B3D1-3CE3C9AF0583}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <v>0.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Move BAU gas processing CCS assumptions into oil and gas 06
</commit_message>
<xml_diff>
--- a/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
+++ b/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\CCP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\CCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7172B8-79FD-4360-98F3-E9249B18DB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C2AF75-4449-4234-82F2-ED89CB505329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1068,7 +1068,9 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C10:C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1115,10 +1117,10 @@
         <v>36</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>